<commit_message>
New functions in Input
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio\C++\Orange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F90CFF-E936-46AD-9484-DA384ED5D14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152587C-E806-4F83-8082-A7E11E0A9238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Shader Class</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>Camera</t>
+  </si>
+  <si>
+    <t>Tiles</t>
+  </si>
+  <si>
+    <t>Tile Class</t>
+  </si>
+  <si>
+    <t>Tileset Class</t>
+  </si>
+  <si>
+    <t>Tilemap Class</t>
   </si>
 </sst>
 </file>
@@ -158,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,6 +180,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -466,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +510,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -509,7 +524,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
@@ -521,7 +536,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -530,7 +545,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -541,7 +556,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -550,7 +565,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -561,7 +576,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
@@ -570,7 +585,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -578,11 +593,32 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{EEA2F99E-DF0D-4614-A08C-F4695B8D98E9}">

</xml_diff>

<commit_message>
DeltaTime in Layer::OnUpdate() function
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio\C++\Orange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F09160-A302-4BB8-BA80-A4AF91FFD90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519A3006-0D0A-49DE-B659-67B0BDF3C108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Shader Class</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>UUID</t>
+  </si>
+  <si>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>FPS; DeltaTime</t>
   </si>
 </sst>
 </file>
@@ -484,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,6 +639,25 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>